<commit_message>
Update .gitignore to exclude __pycache__ and remove cached __pycache__ directories
</commit_message>
<xml_diff>
--- a/data/DunnHumby/DunnHumby.xlsx
+++ b/data/DunnHumby/DunnHumby.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -53,18 +53,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,12 +436,12 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>SFCNTSP</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>DNNTSP</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>SFCNTSP</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -453,52 +453,100 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>weighted f1</t>
+          <t>weighted f1(mean)</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.5016137589360171</v>
+        <v>0.4750733530506966</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3007482299909504</v>
+        <v>0.5059978957473863</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4320323167749578</v>
+        <v>0.5556464286094351</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>weighted ROC AUC</t>
+          <t>weighted f1(std)</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.6562145032369698</v>
+        <v>0.06345638024699643</v>
       </c>
       <c r="C3" t="n">
-        <v>0.5756288929847743</v>
+        <v>0.008413442010530424</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5756288929847743</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>hamming_loss</t>
+          <t>hamming_loss(mean)</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1022727272727273</v>
+        <v>0.106969696969697</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1016363636363636</v>
+        <v>0.1067454545454545</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1066363636363636</v>
+        <v>0.09909090909090909</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>hamming_loss(std)</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.003385541558408321</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.002326562391594835</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>weighted ROC AUC(mean)</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.6080632227869875</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.655800124848401</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.7092846855246081</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>weighted ROC AUC(std)</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.06401437436429813</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.008144567490292331</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>